<commit_message>
Added Pinkbike ErrorTesting Template
Added a new Excel template with commented errors for testing purposes.
</commit_message>
<xml_diff>
--- a/ExcelTemplates/PinkbikeBuySellAllMountain.xlsx
+++ b/ExcelTemplates/PinkbikeBuySellAllMountain.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="25">
   <si>
     <t>Seller</t>
   </si>
@@ -83,9 +83,6 @@
   </si>
   <si>
     <t>element_attribute_value</t>
-  </si>
-  <si>
-    <t>element_content_attribute_name</t>
   </si>
   <si>
     <t>Attribute_Name</t>
@@ -192,8 +189,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -209,15 +208,17 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -547,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40:A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -597,7 +598,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -605,7 +606,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -613,7 +614,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -624,10 +625,10 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -635,7 +636,7 @@
         <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -643,7 +644,7 @@
         <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -651,7 +652,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -662,10 +663,10 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -673,7 +674,7 @@
         <v>7</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -681,7 +682,7 @@
         <v>8</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -693,22 +694,12 @@
     <row r="21" spans="1:2">
       <c r="B21" s="1"/>
     </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s">
-        <v>10</v>
-      </c>
-    </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -716,7 +707,7 @@
         <v>7</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -724,7 +715,7 @@
         <v>8</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -740,10 +731,10 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -751,7 +742,7 @@
         <v>7</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -759,7 +750,7 @@
         <v>8</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -772,10 +763,10 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -783,7 +774,7 @@
         <v>7</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -794,16 +785,6 @@
     <row r="38" spans="1:2">
       <c r="A38" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
-      <c r="A40" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
-      <c r="A41" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>